<commit_message>
Added category column and updated features for the same
</commit_message>
<xml_diff>
--- a/documents/Published/Linear Gauge/LinearGaugeByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Linear Gauge/LinearGaugeByMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18518"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\Linear Gauge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RajveerC\Source\Repos\PowerBI-visuals\documents\Published\Linear Gauge\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A602DF66-6076-41C6-A02C-7F7A2BCD184E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="7965" activeTab="1" xr2:uid="{0699E701-317F-4C2D-BB4C-A0FCB3058AE2}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
   <si>
     <t>S no</t>
   </si>
@@ -45,10 +46,6 @@
     <t>Display basic linear gauge</t>
   </si>
   <si>
-    <t>1. Drag 'Completed' from task table to 'Value'
-2. Drag 'Target' from task table to 'Target value'</t>
-  </si>
-  <si>
     <t>Linear Gauge should be displayed</t>
   </si>
   <si>
@@ -67,12 +64,6 @@
     <t>Drag 'Max Revenue' from store table to 'Maximum value'</t>
   </si>
   <si>
-    <t>Display Targeted value in chart</t>
-  </si>
-  <si>
-    <t>Targeted value will be displayed</t>
-  </si>
-  <si>
     <t>Trend value 1</t>
   </si>
   <si>
@@ -97,28 +88,10 @@
     <t>Starting value will be displayed</t>
   </si>
   <si>
-    <t>Data  label</t>
-  </si>
-  <si>
-    <t>1. Go to formatting pane
-2. Go to 'Data label' option
-3. Update color to 'blue' 
-4. Update display unit to 'Thousand'
-5. Update decimal value  to '1'</t>
-  </si>
-  <si>
-    <t>1. Data label font color will be set to 'Blue'
-2. Text will be formatted like '50K'
-3. Text will be formatted like '50.0K'</t>
-  </si>
-  <si>
     <t>Trend label</t>
   </si>
   <si>
     <t>Update color, display unit and decimal places for trend label</t>
-  </si>
-  <si>
-    <t>Update color, display unit and decimal places for data label</t>
   </si>
   <si>
     <t>1. Go to formatting pane
@@ -128,11 +101,6 @@
 5. Update decimal value  to '3'</t>
   </si>
   <si>
-    <t>1. Data label font color will be set to 'grey'
-2. Text will be formatted like '50K'
-3. Text will be formatted like '50.000K'</t>
-  </si>
-  <si>
     <t># </t>
   </si>
   <si>
@@ -158,9 +126,6 @@
   </si>
   <si>
     <t>Is Selection and Highlight feature working properly by selecting the slice of the visual when we have multiple other visuals along with our visual present in the report? </t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>Does visual work properly on changing format in Modelling ribbon? Should match with other visuals behaviour </t>
@@ -243,12 +208,254 @@
 2. Comparison color in bar will be set to 'red'
 </t>
   </si>
+  <si>
+    <t>Display target  and value  w.r.t. maximum value in chart</t>
+  </si>
+  <si>
+    <t>Position of target marker and value in gauge gets adjusted based on this value</t>
+  </si>
+  <si>
+    <t>Orientation</t>
+  </si>
+  <si>
+    <t>Verify whether orientation is updated or not</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Orientation' option
+3. Update the orientation from Horizontal to Vertical</t>
+  </si>
+  <si>
+    <t>The visual should be displayed in Vertical orientation</t>
+  </si>
+  <si>
+    <t>Target Range</t>
+  </si>
+  <si>
+    <t>Verify whether Target range markers are displayed or not</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Target range' option
+3. Turn on the 'Target range' button
+4. Provide minimum value and maximum value between minimum value and maximum value</t>
+  </si>
+  <si>
+    <t>Target range markers should be displayed on the visual at given minimum and maximum values</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Verify whether Target range marker colors are updated or not</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Target range' option
+3. Turn on the 'Target range' button
+4.  Update the 'Range tick color' to 'Green'</t>
+  </si>
+  <si>
+    <t>Target range minimum and maximum markers should be displayed in 'Green' color</t>
+  </si>
+  <si>
+    <t>Verify whether Scale is displayed or not</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Scale' option
+3. Turn on the 'Scale' button
+4.  Update the 'Tick color' to 'Red'</t>
+  </si>
+  <si>
+    <t>Scale should be displayed in 'Red' color</t>
+  </si>
+  <si>
+    <t>Indicator settings</t>
+  </si>
+  <si>
+    <t>Verify whether Indicator settings are working</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Indicator settings' option
+3. Turn on the 'Indicator settings' button</t>
+  </si>
+  <si>
+    <t>Trend arrows should be displayed in 'Red' color for positive values and 'Green' color for negative values</t>
+  </si>
+  <si>
+    <t>Zone settings</t>
+  </si>
+  <si>
+    <t>Verify whether Zone settings are working</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Zone settings' option
+3. Turn on the 'Zone settings' button</t>
+  </si>
+  <si>
+    <t>Actual value bar will be displayed half of its height in horizontal position and half of its width in vertical position</t>
+  </si>
+  <si>
+    <t>Provide zone values and verify whether zones are created as per provided values</t>
+  </si>
+  <si>
+    <t>The background bar color changes to zone 1 color till zone 1 value on the scale and similarly for other zones</t>
+  </si>
+  <si>
+    <t>Actual value  label</t>
+  </si>
+  <si>
+    <t>Percentage label</t>
+  </si>
+  <si>
+    <t>Verify whether 'Percentage label' settings are working as expected</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Percentage label' option
+3. Update the color to 'Green'
+4. Update the font family to 'Calibri'</t>
+  </si>
+  <si>
+    <t>Percentage label should be displayed in Green color and 'Calibri' font family</t>
+  </si>
+  <si>
+    <t>Update color, display unit and decimal places for actual value label</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Actual value label' option
+3. Update color to 'blue' 
+4. Update display unit to 'Thousand'
+5. Update decimal value  to '1'</t>
+  </si>
+  <si>
+    <t>1. Actual value label font color will be set to 'Blue'
+2. Text will be formatted like '50K'
+3. Text will be formatted like '50.0K'</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Actual value label' option
+3. Update the font family to 'Calibri'</t>
+  </si>
+  <si>
+    <t>Update font family of Actual value label</t>
+  </si>
+  <si>
+    <t>Actual value labels should be displayed in 'calibri' font</t>
+  </si>
+  <si>
+    <t>Update font family of Trend label</t>
+  </si>
+  <si>
+    <t>1. Trend label font color will be set to 'grey'
+2. Text will be formatted like '50K'
+3. Text will be formatted like '50.000K'</t>
+  </si>
+  <si>
+    <t>Trend labels should be displayed in 'Arial' font family</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Trend label' option
+3. Update the font family to 'Arial'</t>
+  </si>
+  <si>
+    <t>1. Drag 'Revenue' from Sales table to 'Actual value'
+2. Drag 'Target' from task table to 'Target value'</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display linear gauge based on categorical column values and legends are created for categorical values </t>
+  </si>
+  <si>
+    <t>Linear Gauge should be divided into different parts based on categorical values</t>
+  </si>
+  <si>
+    <t>Hierarchy</t>
+  </si>
+  <si>
+    <t>Display drill down option on the top of viewport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Drag 'Country' from Sales table to 'Category'
+</t>
+  </si>
+  <si>
+    <t>1. Drag 'Store' from Sales table to 'Category'  
+2. Turn on 'drill down mode' from drill down and click on any legend item</t>
+  </si>
+  <si>
+    <t>1. Drill down feature should be added at the top.
+2. Linear Gauge should display values and gauge for next level of that legend item.</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>Linear Gauge should draw on load</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Animation' option
+3. Turn on the 'Animation option
+4. Provide 4 in Animation time</t>
+  </si>
+  <si>
+    <t>Linear Gauge should draw in 4 second on page load</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Zone settings' option
+3. Turn on the 'Zone settings' button
+4. Select 'Value' from drop down menu.
+5. Provide 350000 in Zone 1 value, 400000 in Zone 2 value, 425000 in Zone 3 value, 450000 in zone 4 value</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Zone settings' option
+3. Turn on the 'Zone settings' button
+4. Select 'Percentage' from drop down menu.
+5. Provide 30 in Zone 1 value, 40 in Zone 2 value, 30 in Zone 3 value</t>
+  </si>
+  <si>
+    <t>Legend Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The background bar color changes to gradient color based on values and colors provided in zone values and zone colors </t>
+  </si>
+  <si>
+    <t>Provide zone percentage and verify whether gradient background color is created as per provided percentage value</t>
+  </si>
+  <si>
+    <t>Update legend color, font size and legend Position</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Category legend' option
+3. Update font size to 15 px
+4. Turn on 'Title' option
+5. Update text color to 'blue'
+6. Update legend position to 'Bottom center'</t>
+  </si>
+  <si>
+    <t>Legend font size  will be set to 15 px
+Legend Title will be displayed before the legend item
+Legend text color set to blue.
+Legend will be displayed at the bottom center position of viewport</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +465,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -306,20 +520,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,16 +865,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D00286-5FAE-4E81-8436-5E389963610F}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="29" style="6" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="45" style="6" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="6"/>
   </cols>
@@ -671,16 +903,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -688,16 +920,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -705,16 +937,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>14</v>
+      <c r="E4" s="9" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -722,16 +954,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -739,16 +971,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -756,53 +988,301 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>8</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>9</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="7" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>10</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="C13" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="E13" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>11</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>12</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>13</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>14</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>15</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>16</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>17</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>18</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -811,279 +1291,271 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34083C1-7852-40FE-85BC-66CC2D6C3381}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="64.7109375" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C6" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C10" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C16" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C17" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C25" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>17</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>18</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>19</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>20</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>35</v>
+      <c r="C26" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>